<commit_message>
#172 upd template position & contractorCode fill
</commit_message>
<xml_diff>
--- a/src/main/resources/template/PurchaseProcedureTemplate.xlsx
+++ b/src/main/resources/template/PurchaseProcedureTemplate.xlsx
@@ -1,102 +1,105 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SalamatinA\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22980" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
-    <t xml:space="preserve">Номер лота</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Идентификатор лота во внутренней системе</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Наименование лота</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Номер процедуры</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Идентификатор процедуры во внутренней системе</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Плановая дата завершения</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Дата публикации</t>
+    <t>Номер лота</t>
+  </si>
+  <si>
+    <t>Идентификатор лота во внутренней системе</t>
+  </si>
+  <si>
+    <t>Наименование лота</t>
+  </si>
+  <si>
+    <t>Номер процедуры</t>
+  </si>
+  <si>
+    <t>Идентификатор процедуры во внутренней системе</t>
+  </si>
+  <si>
+    <t>Плановая дата завершения</t>
+  </si>
+  <si>
+    <t>Дата публикации</t>
   </si>
   <si>
     <t>Организатор</t>
   </si>
   <si>
-    <t xml:space="preserve">Код организатора</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Код инициатора</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Категория закупки</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Форма закупки</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Код услуги</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Код заказчика</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Сумма НМЦ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Дата протокола</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Коды ОКВЭД2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Коды ОКПД2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Код ОКАТО</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Код контрагента во внутренней системе</t>
-  </si>
-  <si>
-    <t xml:space="preserve">наименование поставщика</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Код ЕСУ во внутренней системе</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Инн поставщика</t>
-  </si>
-  <si>
-    <t xml:space="preserve">КПП поставщика</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Сумма контакта</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Дата контракта</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Статус участия</t>
+    <t>Код организатора</t>
+  </si>
+  <si>
+    <t>Код инициатора</t>
+  </si>
+  <si>
+    <t>Категория закупки</t>
+  </si>
+  <si>
+    <t>Форма закупки</t>
+  </si>
+  <si>
+    <t>Код услуги</t>
+  </si>
+  <si>
+    <t>Код заказчика</t>
+  </si>
+  <si>
+    <t>Сумма НМЦ</t>
+  </si>
+  <si>
+    <t>Дата протокола</t>
+  </si>
+  <si>
+    <t>Коды ОКВЭД2</t>
+  </si>
+  <si>
+    <t>Коды ОКПД2</t>
+  </si>
+  <si>
+    <t>Код ОКАТО</t>
+  </si>
+  <si>
+    <t>Код контрагента во внутренней системе</t>
+  </si>
+  <si>
+    <t>наименование поставщика</t>
+  </si>
+  <si>
+    <t>Код ЕСУ во внутренней системе</t>
+  </si>
+  <si>
+    <t>Инн поставщика</t>
+  </si>
+  <si>
+    <t>КПП поставщика</t>
+  </si>
+  <si>
+    <t>Сумма контакта</t>
+  </si>
+  <si>
+    <t>Дата контракта</t>
+  </si>
+  <si>
+    <t>Статус участия</t>
   </si>
   <si>
     <t>lotNr</t>
@@ -183,27 +186,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11.000000"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.000000"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.000000"/>
+      <sz val="11"/>
       <name val="Consolas"/>
     </font>
   </fonts>
@@ -217,26 +217,29 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="2">
     <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -251,27 +254,27 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal style="none"/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf fontId="1" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -291,291 +294,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Angsana New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Cordia New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
     <a:clrScheme name="Стандартная">
       <a:dk1>
@@ -778,47 +498,47 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA100"/>
   <sheetViews>
-    <sheetView topLeftCell="P65" zoomScale="100" workbookViewId="0">
-      <selection activeCell="C14" activeCellId="0" sqref="C14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" min="1" max="1" style="1" width="23.140625"/>
-    <col customWidth="1" min="2" max="2" style="1" width="20"/>
-    <col customWidth="1" min="3" max="3" style="1" width="20.140625"/>
-    <col customWidth="1" min="4" max="4" style="1" width="19.42578125"/>
-    <col customWidth="1" min="5" max="5" style="1" width="29.42578125"/>
-    <col customWidth="1" min="6" max="6" style="1" width="27"/>
-    <col bestFit="1" customWidth="1" min="7" max="7" style="1" width="20.7109375"/>
-    <col bestFit="1" customWidth="1" min="8" max="8" style="1" width="12.5703125"/>
-    <col bestFit="1" customWidth="1" min="9" max="9" style="1" width="17.42578125"/>
-    <col bestFit="1" customWidth="1" min="10" max="10" style="1" width="15.85546875"/>
-    <col bestFit="1" customWidth="1" min="11" max="11" style="1" width="19.5703125"/>
-    <col bestFit="1" customWidth="1" min="12" max="12" style="1" width="14.85546875"/>
-    <col bestFit="1" customWidth="1" min="13" max="13" style="1" width="13.7109375"/>
-    <col bestFit="1" customWidth="1" min="14" max="14" style="1" width="10.140625"/>
-    <col bestFit="1" customWidth="1" min="15" max="15" style="1" width="14.85546875"/>
-    <col bestFit="1" customWidth="1" min="16" max="16" style="1" width="15.5703125"/>
-    <col bestFit="1" customWidth="1" min="17" max="17" style="1" width="13.7109375"/>
-    <col bestFit="1" customWidth="1" min="18" max="18" style="1" width="12.5703125"/>
-    <col bestFit="1" customWidth="1" min="19" max="19" style="1" width="13.7109375"/>
-    <col bestFit="1" customWidth="1" min="20" max="20" style="1" width="30.5703125"/>
-    <col bestFit="1" customWidth="1" min="21" max="21" style="1" width="26.28515625"/>
-    <col bestFit="1" customWidth="1" min="22" max="22" style="1" width="30.5703125"/>
-    <col bestFit="1" customWidth="1" min="23" max="24" style="1" width="16"/>
-    <col bestFit="1" customWidth="1" min="25" max="25" style="1" width="15.5703125"/>
-    <col bestFit="1" customWidth="1" min="26" max="26" style="1" width="15"/>
-    <col bestFit="1" customWidth="1" min="27" max="27" style="1" width="14.140625"/>
+    <col min="1" max="1" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="30.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="60">
+    <row r="1" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -901,7 +621,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
@@ -984,535 +704,533 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" ht="14.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="P3" s="5"/>
       <c r="Z3" s="5"/>
     </row>
-    <row r="4" ht="14.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="P4" s="5"/>
       <c r="Z4" s="5"/>
     </row>
-    <row r="5" ht="14.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="P5" s="5"/>
       <c r="Z5" s="5"/>
     </row>
-    <row r="6" ht="14.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="P6" s="5"/>
       <c r="Z6" s="5"/>
     </row>
-    <row r="7" ht="14.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="P7" s="5"/>
       <c r="Z7" s="5"/>
     </row>
-    <row r="8" ht="14.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="P8" s="5"/>
       <c r="Z8" s="5"/>
     </row>
-    <row r="9" ht="14.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="P9" s="5"/>
       <c r="Z9" s="5"/>
     </row>
-    <row r="10" ht="14.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="P10" s="5"/>
       <c r="Z10" s="5"/>
     </row>
-    <row r="11" ht="14.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="P11" s="5"/>
       <c r="Z11" s="5"/>
     </row>
-    <row r="12" ht="14.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="P12" s="5"/>
       <c r="Z12" s="5"/>
     </row>
-    <row r="13" ht="14.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="P13" s="5"/>
       <c r="Z13" s="5"/>
     </row>
-    <row r="14" ht="14.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="P14" s="5"/>
       <c r="Z14" s="5"/>
     </row>
-    <row r="15" ht="14.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="P15" s="5"/>
       <c r="Z15" s="5"/>
     </row>
-    <row r="16" ht="14.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="P16" s="5"/>
       <c r="Z16" s="5"/>
     </row>
-    <row r="17" ht="14.25">
+    <row r="17" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="P17" s="5"/>
       <c r="Z17" s="5"/>
     </row>
-    <row r="18" ht="14.25">
+    <row r="18" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="P18" s="5"/>
       <c r="Z18" s="5"/>
     </row>
-    <row r="19" ht="14.25">
+    <row r="19" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="P19" s="5"/>
       <c r="Z19" s="5"/>
     </row>
-    <row r="20" ht="14.25">
+    <row r="20" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="P20" s="5"/>
       <c r="Z20" s="5"/>
     </row>
-    <row r="21" ht="14.25">
+    <row r="21" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="P21" s="5"/>
       <c r="Z21" s="5"/>
     </row>
-    <row r="22" ht="14.25">
+    <row r="22" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="P22" s="5"/>
       <c r="Z22" s="5"/>
     </row>
-    <row r="23" ht="14.25">
+    <row r="23" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="P23" s="5"/>
       <c r="Z23" s="5"/>
     </row>
-    <row r="24" ht="14.25">
+    <row r="24" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="P24" s="5"/>
       <c r="Z24" s="5"/>
     </row>
-    <row r="25" ht="14.25">
+    <row r="25" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="P25" s="5"/>
       <c r="Z25" s="5"/>
     </row>
-    <row r="26" ht="14.25">
+    <row r="26" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="P26" s="5"/>
       <c r="Z26" s="5"/>
     </row>
-    <row r="27" ht="14.25">
+    <row r="27" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="P27" s="5"/>
       <c r="Z27" s="5"/>
     </row>
-    <row r="28" ht="14.25">
+    <row r="28" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="P28" s="5"/>
       <c r="Z28" s="5"/>
     </row>
-    <row r="29" ht="14.25">
+    <row r="29" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="P29" s="5"/>
       <c r="Z29" s="5"/>
     </row>
-    <row r="30" ht="14.25">
+    <row r="30" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="P30" s="5"/>
       <c r="Z30" s="5"/>
     </row>
-    <row r="31" ht="14.25">
+    <row r="31" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
       <c r="P31" s="5"/>
       <c r="Z31" s="5"/>
     </row>
-    <row r="32" ht="14.25">
+    <row r="32" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
       <c r="P32" s="5"/>
       <c r="Z32" s="5"/>
     </row>
-    <row r="33" ht="14.25">
+    <row r="33" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
       <c r="P33" s="5"/>
       <c r="Z33" s="5"/>
     </row>
-    <row r="34" ht="14.25">
+    <row r="34" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
       <c r="P34" s="5"/>
       <c r="Z34" s="5"/>
     </row>
-    <row r="35" ht="14.25">
+    <row r="35" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
       <c r="P35" s="5"/>
       <c r="Z35" s="5"/>
     </row>
-    <row r="36" ht="14.25">
+    <row r="36" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
       <c r="P36" s="5"/>
       <c r="Z36" s="5"/>
     </row>
-    <row r="37" ht="14.25">
+    <row r="37" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
       <c r="P37" s="5"/>
       <c r="Z37" s="5"/>
     </row>
-    <row r="38" ht="14.25">
+    <row r="38" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
       <c r="P38" s="5"/>
       <c r="Z38" s="5"/>
     </row>
-    <row r="39" ht="14.25">
+    <row r="39" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
       <c r="P39" s="5"/>
       <c r="Z39" s="5"/>
     </row>
-    <row r="40" ht="14.25">
+    <row r="40" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
       <c r="P40" s="5"/>
       <c r="Z40" s="5"/>
     </row>
-    <row r="41" ht="14.25">
+    <row r="41" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
       <c r="P41" s="5"/>
       <c r="Z41" s="5"/>
     </row>
-    <row r="42" ht="14.25">
+    <row r="42" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
       <c r="P42" s="5"/>
       <c r="Z42" s="5"/>
     </row>
-    <row r="43" ht="14.25">
+    <row r="43" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
       <c r="P43" s="5"/>
       <c r="Z43" s="5"/>
     </row>
-    <row r="44" ht="14.25">
+    <row r="44" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
       <c r="P44" s="5"/>
       <c r="Z44" s="5"/>
     </row>
-    <row r="45" ht="14.25">
+    <row r="45" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
       <c r="P45" s="5"/>
       <c r="Z45" s="5"/>
     </row>
-    <row r="46" ht="14.25">
+    <row r="46" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
       <c r="P46" s="5"/>
       <c r="Z46" s="5"/>
     </row>
-    <row r="47" ht="14.25">
+    <row r="47" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
       <c r="P47" s="5"/>
       <c r="Z47" s="5"/>
     </row>
-    <row r="48" ht="14.25">
+    <row r="48" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
       <c r="P48" s="5"/>
       <c r="Z48" s="5"/>
     </row>
-    <row r="49" ht="14.25">
+    <row r="49" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
       <c r="P49" s="5"/>
       <c r="Z49" s="5"/>
     </row>
-    <row r="50" ht="14.25">
+    <row r="50" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F50" s="5"/>
       <c r="G50" s="5"/>
       <c r="P50" s="5"/>
       <c r="Z50" s="5"/>
     </row>
-    <row r="51" ht="14.25">
+    <row r="51" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>
       <c r="P51" s="5"/>
       <c r="Z51" s="5"/>
     </row>
-    <row r="52" ht="14.25">
+    <row r="52" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F52" s="5"/>
       <c r="G52" s="5"/>
       <c r="P52" s="5"/>
       <c r="Z52" s="5"/>
     </row>
-    <row r="53" ht="14.25">
+    <row r="53" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
       <c r="P53" s="5"/>
       <c r="Z53" s="5"/>
     </row>
-    <row r="54" ht="14.25">
+    <row r="54" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F54" s="5"/>
       <c r="G54" s="5"/>
       <c r="P54" s="5"/>
       <c r="Z54" s="5"/>
     </row>
-    <row r="55" ht="14.25">
+    <row r="55" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F55" s="5"/>
       <c r="G55" s="5"/>
       <c r="P55" s="5"/>
       <c r="Z55" s="5"/>
     </row>
-    <row r="56" ht="14.25">
+    <row r="56" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F56" s="5"/>
       <c r="G56" s="5"/>
       <c r="P56" s="5"/>
       <c r="Z56" s="5"/>
     </row>
-    <row r="57" ht="14.25">
+    <row r="57" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F57" s="5"/>
       <c r="G57" s="5"/>
       <c r="P57" s="5"/>
       <c r="Z57" s="5"/>
     </row>
-    <row r="58" ht="14.25">
+    <row r="58" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
       <c r="P58" s="5"/>
       <c r="Z58" s="5"/>
     </row>
-    <row r="59" ht="14.25">
+    <row r="59" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F59" s="5"/>
       <c r="G59" s="5"/>
       <c r="P59" s="5"/>
       <c r="Z59" s="5"/>
     </row>
-    <row r="60" ht="14.25">
+    <row r="60" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>
       <c r="P60" s="5"/>
       <c r="Z60" s="5"/>
     </row>
-    <row r="61" ht="14.25">
+    <row r="61" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
       <c r="P61" s="5"/>
       <c r="Z61" s="5"/>
     </row>
-    <row r="62" ht="14.25">
+    <row r="62" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F62" s="5"/>
       <c r="G62" s="5"/>
       <c r="P62" s="5"/>
       <c r="Z62" s="5"/>
     </row>
-    <row r="63" ht="14.25">
+    <row r="63" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F63" s="5"/>
       <c r="G63" s="5"/>
       <c r="P63" s="5"/>
       <c r="Z63" s="5"/>
     </row>
-    <row r="64" ht="14.25">
+    <row r="64" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
       <c r="P64" s="5"/>
       <c r="Z64" s="5"/>
     </row>
-    <row r="65" ht="14.25">
+    <row r="65" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F65" s="5"/>
       <c r="G65" s="5"/>
       <c r="P65" s="5"/>
       <c r="Z65" s="5"/>
     </row>
-    <row r="66" ht="14.25">
+    <row r="66" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F66" s="5"/>
       <c r="G66" s="5"/>
       <c r="P66" s="5"/>
       <c r="Z66" s="5"/>
     </row>
-    <row r="67" ht="14.25">
+    <row r="67" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F67" s="5"/>
       <c r="G67" s="5"/>
       <c r="P67" s="5"/>
       <c r="Z67" s="5"/>
     </row>
-    <row r="68" ht="14.25">
+    <row r="68" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F68" s="5"/>
       <c r="G68" s="5"/>
       <c r="P68" s="5"/>
       <c r="Z68" s="5"/>
     </row>
-    <row r="69" ht="14.25">
+    <row r="69" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F69" s="5"/>
       <c r="G69" s="5"/>
       <c r="P69" s="5"/>
       <c r="Z69" s="5"/>
     </row>
-    <row r="70" ht="14.25">
+    <row r="70" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F70" s="5"/>
       <c r="G70" s="5"/>
       <c r="P70" s="5"/>
       <c r="Z70" s="5"/>
     </row>
-    <row r="71" ht="14.25">
+    <row r="71" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F71" s="5"/>
       <c r="G71" s="5"/>
       <c r="P71" s="5"/>
       <c r="Z71" s="5"/>
     </row>
-    <row r="72" ht="14.25">
+    <row r="72" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F72" s="5"/>
       <c r="G72" s="5"/>
       <c r="P72" s="5"/>
       <c r="Z72" s="5"/>
     </row>
-    <row r="73" ht="14.25">
+    <row r="73" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F73" s="5"/>
       <c r="G73" s="5"/>
       <c r="P73" s="5"/>
       <c r="Z73" s="5"/>
     </row>
-    <row r="74" ht="14.25">
+    <row r="74" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F74" s="5"/>
       <c r="G74" s="5"/>
       <c r="P74" s="5"/>
       <c r="Z74" s="5"/>
     </row>
-    <row r="75" ht="14.25">
+    <row r="75" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F75" s="5"/>
       <c r="G75" s="5"/>
       <c r="P75" s="5"/>
       <c r="Z75" s="5"/>
     </row>
-    <row r="76" ht="14.25">
+    <row r="76" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F76" s="5"/>
       <c r="G76" s="5"/>
       <c r="P76" s="5"/>
       <c r="Z76" s="5"/>
     </row>
-    <row r="77" ht="14.25">
+    <row r="77" spans="6:26" x14ac:dyDescent="0.25">
       <c r="G77" s="5"/>
       <c r="P77" s="5"/>
       <c r="Z77" s="5"/>
     </row>
-    <row r="78" ht="14.25">
+    <row r="78" spans="6:26" x14ac:dyDescent="0.25">
       <c r="G78" s="5"/>
       <c r="P78" s="5"/>
       <c r="Z78" s="5"/>
     </row>
-    <row r="79" ht="14.25">
+    <row r="79" spans="6:26" x14ac:dyDescent="0.25">
       <c r="G79" s="5"/>
       <c r="P79" s="5"/>
       <c r="Z79" s="5"/>
     </row>
-    <row r="80" ht="14.25">
+    <row r="80" spans="6:26" x14ac:dyDescent="0.25">
       <c r="G80" s="5"/>
       <c r="P80" s="5"/>
       <c r="Z80" s="5"/>
     </row>
-    <row r="81" ht="14.25">
+    <row r="81" spans="16:26" x14ac:dyDescent="0.25">
       <c r="P81" s="5"/>
       <c r="Z81" s="5"/>
     </row>
-    <row r="82" ht="14.25">
+    <row r="82" spans="16:26" x14ac:dyDescent="0.25">
       <c r="Z82" s="5"/>
     </row>
-    <row r="83" ht="14.25">
+    <row r="83" spans="16:26" x14ac:dyDescent="0.25">
       <c r="Z83" s="5"/>
     </row>
-    <row r="84" ht="14.25">
+    <row r="84" spans="16:26" x14ac:dyDescent="0.25">
       <c r="Z84" s="5"/>
     </row>
-    <row r="85" ht="14.25">
+    <row r="85" spans="16:26" x14ac:dyDescent="0.25">
       <c r="Z85" s="5"/>
     </row>
-    <row r="86" ht="14.25">
+    <row r="86" spans="16:26" x14ac:dyDescent="0.25">
       <c r="Z86" s="5"/>
     </row>
-    <row r="87" ht="14.25">
+    <row r="87" spans="16:26" x14ac:dyDescent="0.25">
       <c r="Z87" s="5"/>
     </row>
-    <row r="88" ht="14.25">
+    <row r="88" spans="16:26" x14ac:dyDescent="0.25">
       <c r="Z88" s="5"/>
     </row>
-    <row r="89" ht="14.25">
+    <row r="89" spans="16:26" x14ac:dyDescent="0.25">
       <c r="Z89" s="5"/>
     </row>
-    <row r="90" ht="14.25">
+    <row r="90" spans="16:26" x14ac:dyDescent="0.25">
       <c r="Z90" s="5"/>
     </row>
-    <row r="91" ht="14.25">
+    <row r="91" spans="16:26" x14ac:dyDescent="0.25">
       <c r="Z91" s="5"/>
     </row>
-    <row r="92" ht="14.25">
+    <row r="92" spans="16:26" x14ac:dyDescent="0.25">
       <c r="Z92" s="5"/>
     </row>
-    <row r="93" ht="14.25">
+    <row r="93" spans="16:26" x14ac:dyDescent="0.25">
       <c r="Z93" s="5"/>
     </row>
-    <row r="94" ht="14.25">
+    <row r="94" spans="16:26" x14ac:dyDescent="0.25">
       <c r="Z94" s="5"/>
     </row>
-    <row r="95" ht="14.25">
+    <row r="95" spans="16:26" x14ac:dyDescent="0.25">
       <c r="Z95" s="5"/>
     </row>
-    <row r="96" ht="14.25">
+    <row r="96" spans="16:26" x14ac:dyDescent="0.25">
       <c r="Z96" s="5"/>
     </row>
-    <row r="97" ht="14.25">
+    <row r="97" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z97" s="5"/>
     </row>
-    <row r="98" ht="14.25">
+    <row r="98" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z98" s="5"/>
     </row>
-    <row r="99" ht="14.25">
+    <row r="99" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z99" s="5"/>
     </row>
-    <row r="100" ht="14.25">
+    <row r="100" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z100" s="5"/>
     </row>
   </sheetData>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>